<commit_message>
Add shifter test cases
</commit_message>
<xml_diff>
--- a/50002_1d/TestCases.xlsx
+++ b/50002_1d/TestCases.xlsx
@@ -1,27 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanleynguyen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tadityar/Work/programming/school/50.002/50002_1d/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="27320" windowHeight="14840" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Add8" sheetId="1" r:id="rId1"/>
     <sheet name="Comp8" sheetId="2" r:id="rId2"/>
     <sheet name="Bool8" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Shift8" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="93">
   <si>
     <t>1 to 8</t>
   </si>
@@ -216,6 +213,99 @@
   </si>
   <si>
     <t>11101110</t>
+  </si>
+  <si>
+    <t>ALUFN1</t>
+  </si>
+  <si>
+    <t>ALUFN0</t>
+  </si>
+  <si>
+    <t>00000010</t>
+  </si>
+  <si>
+    <t>00000100</t>
+  </si>
+  <si>
+    <t>11001111</t>
+  </si>
+  <si>
+    <t>01110100</t>
+  </si>
+  <si>
+    <t>00000011</t>
+  </si>
+  <si>
+    <t>00000111</t>
+  </si>
+  <si>
+    <t>10100110</t>
+  </si>
+  <si>
+    <t>00010101</t>
+  </si>
+  <si>
+    <t>11110100</t>
+  </si>
+  <si>
+    <t>This test case includes 0,-1,-128,127, and 2 random integers</t>
+  </si>
+  <si>
+    <t>11111100</t>
+  </si>
+  <si>
+    <t>11110000</t>
+  </si>
+  <si>
+    <t>10011110</t>
+  </si>
+  <si>
+    <t>01111000</t>
+  </si>
+  <si>
+    <t>11101000</t>
+  </si>
+  <si>
+    <t>10100000</t>
+  </si>
+  <si>
+    <t>00111111</t>
+  </si>
+  <si>
+    <t>00001111</t>
+  </si>
+  <si>
+    <t>01000000</t>
+  </si>
+  <si>
+    <t>00100000</t>
+  </si>
+  <si>
+    <t>00001000</t>
+  </si>
+  <si>
+    <t>00011111</t>
+  </si>
+  <si>
+    <t>01010011</t>
+  </si>
+  <si>
+    <t>00010100</t>
+  </si>
+  <si>
+    <t>00001010</t>
+  </si>
+  <si>
+    <t>11000000</t>
+  </si>
+  <si>
+    <t>11100000</t>
+  </si>
+  <si>
+    <t>11111000</t>
+  </si>
+  <si>
+    <t>11111010</t>
   </si>
 </sst>
 </file>
@@ -371,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -388,6 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +759,7 @@
   <dimension ref="A3:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1109,7 +1200,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1560,7 +1651,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1802,12 +1893,1267 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="8" max="8" width="49.5" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="14">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="14">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="14">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="14">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="14">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="14">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="14">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="14">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="14">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="14">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="14">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="14">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="14">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="14">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="14">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="14">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="14">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="14">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="14">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="14">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="14">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="14">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="14">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="14">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="14">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="14">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="14">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="14">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="14">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="14">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="14">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="14">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="14">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="14">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="14">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="14">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="14">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="14">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="14">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="14">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="14">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="14">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="14">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="14">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="14">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="14">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="14">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="14">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="14">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="14">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="14">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="14">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="14">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testcases for add in rom
</commit_message>
<xml_diff>
--- a/50002_1d/TestCases.xlsx
+++ b/50002_1d/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Add8" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="119">
   <si>
     <t>out</t>
   </si>
@@ -71,9 +71,6 @@
     <t>00000000</t>
   </si>
   <si>
-    <t>invalid</t>
-  </si>
-  <si>
     <t>10111110</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>10100100</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>10011100</t>
   </si>
   <si>
@@ -390,6 +384,9 @@
   </si>
   <si>
     <t>01001011</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -874,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L32"/>
+  <dimension ref="A3:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,13 +892,13 @@
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -916,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="9"/>
@@ -947,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="12"/>
@@ -1067,22 +1064,22 @@
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1092,23 +1089,23 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
+      <c r="C11" s="6">
+        <v>10000000</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>11111111</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1118,23 +1115,23 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
+      <c r="C12">
+        <v>10000000</v>
+      </c>
+      <c r="D12">
+        <v>10010110</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1144,23 +1141,23 @@
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13" s="6">
-        <v>10000000</v>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>11111111</v>
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1170,23 +1167,23 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
-        <v>10000000</v>
-      </c>
-      <c r="D14">
-        <v>10010110</v>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1197,22 +1194,22 @@
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1222,14 +1219,14 @@
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>85</v>
+      <c r="C16">
+        <v>10000000</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="E16">
+        <v>10101011</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1238,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1246,25 +1243,25 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>91</v>
+        <v>6</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>92</v>
+      <c r="G17">
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1272,16 +1269,16 @@
         <v>14</v>
       </c>
       <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>10000000</v>
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18">
-        <v>10101011</v>
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1290,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1301,19 +1298,19 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1327,19 +1324,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1353,19 +1350,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1379,22 +1376,22 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1404,20 +1401,20 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="6">
+        <v>10000000</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1431,13 +1428,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1446,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1457,16 +1454,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1483,16 +1480,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1508,20 +1505,20 @@
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="6">
-        <v>10000000</v>
+      <c r="C27" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1535,125 +1532,21 @@
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>25</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>26</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>27</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>28</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
         <v>1</v>
       </c>
     </row>
@@ -1683,7 +1576,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1700,7 +1593,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1715,12 +1608,12 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1735,12 +1628,12 @@
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1757,7 +1650,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1774,7 +1667,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1791,7 +1684,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1808,7 +1701,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1825,7 +1718,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1842,7 +1735,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1859,7 +1752,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1876,7 +1769,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1893,7 +1786,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1910,7 +1803,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1927,7 +1820,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1944,7 +1837,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1961,7 +1854,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1978,7 +1871,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1995,7 +1888,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2012,7 +1905,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -2029,7 +1922,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -2046,7 +1939,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2063,7 +1956,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2080,7 +1973,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2097,7 +1990,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2135,27 +2028,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -2163,195 +2056,195 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>7</v>
@@ -2359,55 +2252,55 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1">
         <v>10100011</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -2415,58 +2308,58 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1">
         <v>10110100</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2478,7 +2371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -2491,19 +2384,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2523,7 +2416,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2543,7 +2436,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2557,7 +2450,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
@@ -2574,7 +2467,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -2625,10 +2518,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2642,10 +2535,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2693,7 +2586,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
@@ -2710,7 +2603,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
@@ -2761,10 +2654,10 @@
         <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2778,10 +2671,10 @@
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2792,13 +2685,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2809,13 +2702,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2826,13 +2719,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2843,10 +2736,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>9</v>
@@ -2860,13 +2753,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2877,13 +2770,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2894,13 +2787,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2911,10 +2804,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
@@ -2965,7 +2858,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
@@ -2982,7 +2875,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
@@ -3033,10 +2926,10 @@
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3050,10 +2943,10 @@
         <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -3087,7 +2980,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -3101,10 +2994,10 @@
         <v>9</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -3118,10 +3011,10 @@
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -3155,7 +3048,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -3169,10 +3062,10 @@
         <v>10</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -3186,10 +3079,10 @@
         <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -3200,13 +3093,13 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -3217,13 +3110,13 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -3234,13 +3127,13 @@
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -3251,10 +3144,10 @@
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>11</v>
@@ -3268,13 +3161,13 @@
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -3285,13 +3178,13 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -3302,13 +3195,13 @@
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -3319,10 +3212,10 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>12</v>
@@ -3373,7 +3266,7 @@
         <v>12</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>12</v>
@@ -3390,7 +3283,7 @@
         <v>12</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>12</v>
@@ -3441,7 +3334,7 @@
         <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>7</v>
@@ -3458,7 +3351,7 @@
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>7</v>
@@ -3495,7 +3388,7 @@
         <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -3509,10 +3402,10 @@
         <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -3526,10 +3419,10 @@
         <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -3563,7 +3456,7 @@
         <v>11</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -3577,10 +3470,10 @@
         <v>10</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -3594,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -3608,13 +3501,13 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -3625,13 +3518,13 @@
         <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -3642,10 +3535,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>8</v>
@@ -3659,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>7</v>
@@ -3676,13 +3569,13 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -3693,13 +3586,13 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -3710,13 +3603,13 @@
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -3727,10 +3620,10 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>

</xml_diff>